<commit_message>
Update DateBase/orders/Kanara Greens and Flowers Trading_2024-9-24.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Kanara Greens and Flowers Trading_2024-9-24.xlsx
+++ b/DateBase/orders/Kanara Greens and Flowers Trading_2024-9-24.xlsx
@@ -445,6 +445,9 @@
       <c r="C2" t="str">
         <v>1_白洋桔梗_White Lisianthus_Eustoma Salisb.</v>
       </c>
+      <c r="F2" t="str">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -502,8 +505,8 @@
       <c r="F2" t="str">
         <v>0.00</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="str">
+        <v>01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>